<commit_message>
Prepare public release and harden processing reliability
</commit_message>
<xml_diff>
--- a/tests/performance/batch_100_files/xlsx/xlsx_001.xlsx
+++ b/tests/performance/batch_100_files/xlsx/xlsx_001.xlsx
@@ -7,7 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,28 +426,65 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Data1</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Value</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>123</t>
+          <t>Value1</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Data2</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Value2</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>